<commit_message>
wireframes, text and domain model added
</commit_message>
<xml_diff>
--- a/modèle de domaine.xlsx
+++ b/modèle de domaine.xlsx
@@ -12,29 +12,14 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$G$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$F$49</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
-  <si>
-    <t>Mentoré</t>
-  </si>
-  <si>
-    <t>prénom : String</t>
-  </si>
-  <si>
-    <t>nom : String</t>
-  </si>
-  <si>
-    <t>dateNaissance : String</t>
-  </si>
-  <si>
-    <t>Calendrier</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>rappelNotifications : String</t>
   </si>
@@ -42,12 +27,6 @@
     <t>Mentor</t>
   </si>
   <si>
-    <t>Sexe : String</t>
-  </si>
-  <si>
-    <t>competenceAborde : String (list)</t>
-  </si>
-  <si>
     <t>competenceValide : String (list)</t>
   </si>
   <si>
@@ -57,82 +36,118 @@
     <t>graphMonteeEnCompetence : integer</t>
   </si>
   <si>
-    <t>MesureUtilisation</t>
-  </si>
-  <si>
-    <t>nombreConnexion : integer</t>
-  </si>
-  <si>
     <t>dateConnexion : String</t>
   </si>
   <si>
-    <t>lienVersAppDeWebCam : String</t>
-  </si>
-  <si>
-    <t>noteEnCoursDeSession : String</t>
-  </si>
-  <si>
-    <t>nomPrenomMentor : String (list)</t>
-  </si>
-  <si>
-    <t>nomPrenomMentore : String (list)</t>
-  </si>
-  <si>
     <t>appreciationUtilisateur : integer</t>
   </si>
   <si>
     <t>retourEtCommentairesUtilisateur : String</t>
   </si>
   <si>
-    <t>envoiMail : String</t>
-  </si>
-  <si>
     <t>graphiqueConnexion : integer</t>
   </si>
   <si>
     <t>courbeDeProgression : integer</t>
   </si>
   <si>
-    <t>metierActuel : String</t>
-  </si>
-  <si>
-    <t>nombreAnneesExperienceDomaine : integer</t>
-  </si>
-  <si>
-    <t>estDejaMentore : boolean</t>
-  </si>
-  <si>
-    <t>avezVousDejaMentore : boolean</t>
-  </si>
-  <si>
-    <t>nbreAnneeDeMentorat : integer</t>
-  </si>
-  <si>
-    <t>recommanderAUnTier : boolean</t>
-  </si>
-  <si>
     <t>mailTier : String</t>
   </si>
   <si>
-    <t>enregistrementDeSession : boolean</t>
-  </si>
-  <si>
-    <t>Identité</t>
-  </si>
-  <si>
-    <t>idConnexion : String</t>
-  </si>
-  <si>
-    <t>connaissanceAcquiseOuSouhait : String(List)</t>
-  </si>
-  <si>
-    <t>Recommendation</t>
-  </si>
-  <si>
     <t>dateRdv : DateTime</t>
   </si>
   <si>
     <t>dateConnexion : DateTime</t>
+  </si>
+  <si>
+    <t>id : integer</t>
+  </si>
+  <si>
+    <t>LogUtilisation</t>
+  </si>
+  <si>
+    <t>appreciationSession : integer</t>
+  </si>
+  <si>
+    <t>noteDeProgression : integer</t>
+  </si>
+  <si>
+    <t>typeConnexion : enum (web , mobile)</t>
+  </si>
+  <si>
+    <t>LogRecommendation</t>
+  </si>
+  <si>
+    <t>id utilisateur</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Type : enum (visio ou présentiel)</t>
+  </si>
+  <si>
+    <t>motDePasse : String</t>
+  </si>
+  <si>
+    <t>Mentee</t>
+  </si>
+  <si>
+    <t>actualProfession : String</t>
+  </si>
+  <si>
+    <t>sex : String</t>
+  </si>
+  <si>
+    <t>birthDate: DateTime</t>
+  </si>
+  <si>
+    <t>userName : String</t>
+  </si>
+  <si>
+    <t>lastName : String</t>
+  </si>
+  <si>
+    <t>fisrtName : String</t>
+  </si>
+  <si>
+    <t>haveYouAlreadyTeach : boolean</t>
+  </si>
+  <si>
+    <t>numberYearsTeaching : integer</t>
+  </si>
+  <si>
+    <t>acquiredKnowledgeOrWish : String(List)</t>
+  </si>
+  <si>
+    <t>experienceNumberYears : integer</t>
+  </si>
+  <si>
+    <t>haveYouAlreadyAMentor : boolean</t>
+  </si>
+  <si>
+    <t>mailUser : String</t>
+  </si>
+  <si>
+    <t>Appreciation</t>
+  </si>
+  <si>
+    <t>connexionNumber : integer</t>
+  </si>
+  <si>
+    <t>skillSeen: String (list)</t>
+  </si>
+  <si>
+    <t>camLinkOrMeet : String</t>
+  </si>
+  <si>
+    <t>sessionNote : String</t>
+  </si>
+  <si>
+    <t>registeredSession : boolean</t>
+  </si>
+  <si>
+    <t>Identity</t>
   </si>
 </sst>
 </file>
@@ -207,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -225,6 +240,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -238,70 +268,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2677033</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>188671</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>14383</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>134000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1119535</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>83896</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Flèche droite 7"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="2488576">
-          <a:off x="2753233" y="2893771"/>
-          <a:ext cx="2395377" cy="276225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1758179</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>25745</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>244195</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>111470</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>290608</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76881</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -309,117 +285,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="8222672">
-          <a:off x="5787254" y="2921345"/>
-          <a:ext cx="2276966" cy="276225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19559</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>45796</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>131521</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Flèche droite 9"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3000884" y="1217371"/>
-          <a:ext cx="1028192" cy="276225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2734184</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>55321</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1019176</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>141046</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Flèche droite 10"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="6763259" y="845896"/>
-          <a:ext cx="1028192" cy="276225"/>
+        <a:xfrm rot="7563576">
+          <a:off x="5411523" y="2870382"/>
+          <a:ext cx="3032294" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -455,13 +323,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>509</xdr:colOff>
+      <xdr:colOff>17073</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>93421</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1028701</xdr:colOff>
+      <xdr:colOff>1045265</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>179146</xdr:rowOff>
     </xdr:to>
@@ -472,61 +340,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6772784" y="1264996"/>
-          <a:ext cx="1028192" cy="276225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2896109</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>45796</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1019176</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>131521</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Flèche droite 12"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="2972309" y="836371"/>
+          <a:off x="6792247" y="1261269"/>
           <a:ext cx="1028192" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -564,13 +378,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2495124</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>162096</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2859654</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>122005</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -618,13 +432,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2217607</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>69237</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2299680</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>52767</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -672,13 +486,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1590674</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -723,13 +537,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2238375</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -774,15 +588,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1600200</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:colOff>1548848</xdr:colOff>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>1588</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -790,9 +604,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1676400" y="8124825"/>
-          <a:ext cx="2362200" cy="9526"/>
+        <a:xfrm>
+          <a:off x="1623391" y="8481391"/>
+          <a:ext cx="2419764" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -823,16 +637,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2693096</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>33131</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>723903</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>9527</xdr:rowOff>
+      <xdr:colOff>745436</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>34375</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -840,9 +654,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="6781801" y="8134351"/>
-          <a:ext cx="1762127" cy="1"/>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="6726726" y="8514522"/>
+          <a:ext cx="1845775" cy="1244"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -869,6 +683,222 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19559</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128622</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>32129</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Flèche droite 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3001298" y="1296470"/>
+          <a:ext cx="1032333" cy="284507"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2901907</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>136905</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1027044</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>32129</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Flèche droite 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="2976450" y="724970"/>
+          <a:ext cx="1032333" cy="284507"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6306</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>131936</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1038639</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>27160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Flèche droite 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="6781480" y="720001"/>
+          <a:ext cx="1032333" cy="284507"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>485560</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>68891</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>761785</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>77776</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Flèche droite 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="3785609">
+          <a:off x="2250904" y="2834134"/>
+          <a:ext cx="2709015" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1159,274 +1189,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F44"/>
+  <dimension ref="B2:H50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="1.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="41.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1">
+    <row r="2" spans="2:8" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:8" ht="15.75" thickBot="1">
       <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B10" s="11"/>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="11"/>
+      <c r="D11" s="2"/>
+      <c r="H11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="11"/>
+      <c r="D12" s="2"/>
+      <c r="H12" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="11"/>
+      <c r="D13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B14" s="11"/>
+      <c r="D14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="11"/>
+      <c r="D15" s="8"/>
+      <c r="H15" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="11"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="11"/>
+      <c r="H17" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="11"/>
+      <c r="H18" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="11"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="11"/>
+      <c r="H20" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="H21" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" thickBot="1">
+      <c r="H22" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="2" t="s">
+    <row r="23" spans="2:8" ht="15.75" thickBot="1">
+      <c r="D23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="D24" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="D25" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="D26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="D27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="D28" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="D30" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="D31" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="D32" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="21" spans="2:6" ht="15.75" thickBot="1">
-      <c r="D21" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="D22" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="D23" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="D24" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="D25" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="D27" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="D28" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="D29" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="D30" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="15.75" thickBot="1">
-      <c r="D31" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="33" spans="4:4" ht="15.75" thickBot="1">
-      <c r="D33" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="D35" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4">
-      <c r="D36" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="D37" s="2" t="s">
-        <v>20</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" ht="15.75" thickBot="1">
+      <c r="D35" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" ht="15.75" thickBot="1"/>
+    <row r="37" spans="4:4" ht="15.75" thickBot="1">
+      <c r="D37" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="4:4">
       <c r="D38" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="D40" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="4:4" ht="15.75" thickBot="1">
-      <c r="D39" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4" ht="15.75" thickBot="1"/>
-    <row r="42" spans="4:4" ht="15.75" thickBot="1">
-      <c r="D42" s="6" t="s">
-        <v>35</v>
+    <row r="41" spans="4:4">
+      <c r="D41" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4">
+      <c r="D42" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="4:4">
       <c r="D43" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="4:4" ht="15.75" thickBot="1">
-      <c r="D44" s="3" t="s">
-        <v>30</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4">
+      <c r="D44" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" ht="15.75" thickBot="1">
+      <c r="D45" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" ht="15.75" thickBot="1"/>
+    <row r="48" spans="4:4" ht="15.75" thickBot="1">
+      <c r="D48" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="D49" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" ht="15.75" thickBot="1">
+      <c r="D50" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>